<commit_message>
Add notes from 2016 plot setup at CFCT, CFNT
</commit_message>
<xml_diff>
--- a/data/Plot locations.xlsx
+++ b/data/Plot locations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
   <si>
     <t>Year</t>
   </si>
@@ -111,9 +111,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -139,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +149,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,26 +188,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -209,7 +200,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -519,23 +534,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -570,21 +585,21 @@
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="14">
         <v>2012</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="3">
@@ -599,19 +614,19 @@
       <c r="F4" s="3">
         <v>-117.08089</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="12">
         <v>41046</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="12">
         <v>41138</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3">
         <v>2</v>
       </c>
@@ -624,13 +639,13 @@
       <c r="F5" s="3">
         <v>-117.08078999999999</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="3">
         <v>3</v>
       </c>
@@ -643,13 +658,13 @@
       <c r="F6" s="3">
         <v>-117.08054</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="3">
         <v>4</v>
       </c>
@@ -662,13 +677,13 @@
       <c r="F7" s="3">
         <v>-117.08132000000001</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1">
@@ -683,16 +698,16 @@
       <c r="F8" s="1">
         <v>-117.07777</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>41046</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="13">
         <v>41138</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="1">
         <v>2</v>
       </c>
@@ -705,12 +720,12 @@
       <c r="F9" s="1">
         <v>-117.07767</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="1">
         <v>3</v>
       </c>
@@ -723,12 +738,12 @@
       <c r="F10" s="1">
         <v>-117.07746</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="1">
         <v>4</v>
       </c>
@@ -741,14 +756,14 @@
       <c r="F11" s="1">
         <v>-117.07822</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="15">
         <v>2013</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3">
@@ -763,16 +778,16 @@
       <c r="F12" s="3">
         <v>-117.08068</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="12">
         <v>41453</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="12">
         <v>41528</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="3">
         <v>2</v>
       </c>
@@ -785,12 +800,12 @@
       <c r="F13" s="3">
         <v>-117.08068</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="3">
         <v>3</v>
       </c>
@@ -803,12 +818,12 @@
       <c r="F14" s="3">
         <v>-117.08110000000001</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="3">
         <v>4</v>
       </c>
@@ -821,12 +836,12 @@
       <c r="F15" s="3">
         <v>-117.08029000000001</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1">
@@ -841,16 +856,16 @@
       <c r="F16" s="1">
         <v>-117.07765000000001</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="13">
         <v>41453</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="13">
         <v>41528</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="1">
         <v>2</v>
       </c>
@@ -863,12 +878,12 @@
       <c r="F17" s="1">
         <v>-117.07765000000001</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="1">
         <v>3</v>
       </c>
@@ -881,12 +896,12 @@
       <c r="F18" s="1">
         <v>-117.07805</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="1">
         <v>4</v>
       </c>
@@ -899,12 +914,12 @@
       <c r="F19" s="1">
         <v>-117.07738999999999</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="3">
@@ -919,19 +934,19 @@
       <c r="F20" s="3">
         <v>-118.59832</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="12">
         <v>41408</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="12">
         <v>41487</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="3">
         <v>2</v>
       </c>
@@ -944,13 +959,13 @@
       <c r="F21" s="3">
         <v>-118.59828</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="3">
         <v>3</v>
       </c>
@@ -963,13 +978,13 @@
       <c r="F22" s="3">
         <v>-118.59793000000001</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="3">
         <v>4</v>
       </c>
@@ -982,13 +997,13 @@
       <c r="F23" s="3">
         <v>-118.59872</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1">
@@ -1003,19 +1018,19 @@
       <c r="F24" s="1">
         <v>-116.94855</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="13">
         <v>41415</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="13">
         <v>41506</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="1">
         <v>2</v>
       </c>
@@ -1028,13 +1043,13 @@
       <c r="F25" s="1">
         <v>-116.94853999999999</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="12"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="1">
         <v>3</v>
       </c>
@@ -1047,13 +1062,13 @@
       <c r="F26" s="1">
         <v>-116.94815</v>
       </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="12"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="1">
         <v>4</v>
       </c>
@@ -1066,15 +1081,15 @@
       <c r="F27" s="1">
         <v>-116.94896</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="12"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="14">
         <v>2014</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="3">
@@ -1089,19 +1104,19 @@
       <c r="F28" s="3">
         <v>-117.08078</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="12">
         <v>41748</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="12">
         <v>41853</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="3">
         <v>2</v>
       </c>
@@ -1114,13 +1129,13 @@
       <c r="F29" s="3">
         <v>-117.08089</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="3">
         <v>3</v>
       </c>
@@ -1133,13 +1148,13 @@
       <c r="F30" s="3">
         <v>-117.08138</v>
       </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="3">
         <v>4</v>
       </c>
@@ -1152,13 +1167,13 @@
       <c r="F31" s="3">
         <v>-117.08051</v>
       </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="7" t="s">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="1">
@@ -1173,19 +1188,19 @@
       <c r="F32" s="1">
         <v>-117.07764</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="13">
         <v>41748</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="13">
         <v>41853</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="I32" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="1">
         <v>2</v>
       </c>
@@ -1198,13 +1213,13 @@
       <c r="F33" s="1">
         <v>-117.07767</v>
       </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="12"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="1">
         <v>3</v>
       </c>
@@ -1217,13 +1232,13 @@
       <c r="F34" s="1">
         <v>-117.07813</v>
       </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="12"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="1">
         <v>4</v>
       </c>
@@ -1236,13 +1251,13 @@
       <c r="F35" s="1">
         <v>-117.0775</v>
       </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="12"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="3">
@@ -1257,16 +1272,16 @@
       <c r="F36" s="3">
         <v>-116.94868</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="12">
         <v>41813</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="12">
         <v>41857</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="3">
         <v>2</v>
       </c>
@@ -1279,12 +1294,12 @@
       <c r="F37" s="3">
         <v>-116.94832</v>
       </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="3">
         <v>3</v>
       </c>
@@ -1297,12 +1312,12 @@
       <c r="F38" s="3">
         <v>-116.94914</v>
       </c>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="3">
         <v>4</v>
       </c>
@@ -1315,12 +1330,12 @@
       <c r="F39" s="3">
         <v>-116.94839</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="3" t="s">
         <v>11</v>
       </c>
@@ -1333,12 +1348,12 @@
       <c r="F40" s="3">
         <v>-116.94785</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="3" t="s">
         <v>12</v>
       </c>
@@ -1351,12 +1366,12 @@
       <c r="F41" s="3">
         <v>-116.94764000000001</v>
       </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="3" t="s">
         <v>13</v>
       </c>
@@ -1369,14 +1384,14 @@
       <c r="F42" s="3">
         <v>-116.94743</v>
       </c>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+      <c r="A43" s="15">
         <v>2015</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="1">
@@ -1391,19 +1406,19 @@
       <c r="F43" s="1">
         <v>-117.08078</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G43" s="13">
         <v>42142</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43" s="13">
         <v>42226</v>
       </c>
-      <c r="I43" s="12" t="s">
+      <c r="I43" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="1">
         <v>2</v>
       </c>
@@ -1416,13 +1431,13 @@
       <c r="F44" s="1">
         <v>-117.08083000000001</v>
       </c>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="12"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="1">
         <v>3</v>
       </c>
@@ -1435,13 +1450,13 @@
       <c r="F45" s="1">
         <v>-117.08125</v>
       </c>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="12"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="1">
         <v>4</v>
       </c>
@@ -1454,13 +1469,13 @@
       <c r="F46" s="1">
         <v>-117.08045</v>
       </c>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="12"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="5" t="s">
+      <c r="A47" s="15"/>
+      <c r="B47" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="3">
@@ -1475,19 +1490,19 @@
       <c r="F47" s="3">
         <v>-117.07762</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="12">
         <v>42142</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="12">
         <v>42226</v>
       </c>
-      <c r="I47" s="12" t="s">
+      <c r="I47" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="3">
         <v>2</v>
       </c>
@@ -1500,13 +1515,13 @@
       <c r="F48" s="3">
         <v>-117.07758</v>
       </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="14"/>
       <c r="C49" s="3">
         <v>3</v>
       </c>
@@ -1519,13 +1534,13 @@
       <c r="F49" s="3">
         <v>-117.07792999999999</v>
       </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="14"/>
       <c r="C50" s="3">
         <v>4</v>
       </c>
@@ -1538,13 +1553,13 @@
       <c r="F50" s="3">
         <v>-117.07735</v>
       </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="15"/>
+      <c r="B51" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="1">
@@ -1559,19 +1574,19 @@
       <c r="F51" s="1">
         <v>-118.59838999999999</v>
       </c>
-      <c r="G51" s="15">
+      <c r="G51" s="13">
         <v>42082</v>
       </c>
-      <c r="H51" s="15">
+      <c r="H51" s="13">
         <v>42194</v>
       </c>
-      <c r="I51" s="12" t="s">
+      <c r="I51" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="1">
         <v>2</v>
       </c>
@@ -1584,13 +1599,13 @@
       <c r="F52" s="1">
         <v>-118.5984</v>
       </c>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="12"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="10"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="1">
         <v>3</v>
       </c>
@@ -1603,13 +1618,13 @@
       <c r="F53" s="1">
         <v>-118.59878999999999</v>
       </c>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="12"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="10"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
       <c r="C54" s="1">
         <v>4</v>
       </c>
@@ -1622,13 +1637,13 @@
       <c r="F54" s="1">
         <v>-118.59805</v>
       </c>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="12"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="10"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="5" t="s">
+      <c r="A55" s="15"/>
+      <c r="B55" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C55" s="3">
@@ -1643,16 +1658,16 @@
       <c r="F55" s="3">
         <v>-116.94859</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="12">
         <v>42090</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H55" s="12">
         <v>42219</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="5"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="14"/>
       <c r="C56" s="3">
         <v>2</v>
       </c>
@@ -1665,12 +1680,12 @@
       <c r="F56" s="3">
         <v>-116.94879</v>
       </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="5"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="14"/>
       <c r="C57" s="3">
         <v>3</v>
       </c>
@@ -1683,12 +1698,12 @@
       <c r="F57" s="3">
         <v>-116.94925000000001</v>
       </c>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="5"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="14"/>
       <c r="C58" s="3">
         <v>4</v>
       </c>
@@ -1701,41 +1716,186 @@
       <c r="F58" s="3">
         <v>-116.94855</v>
       </c>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <v>2016</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="17">
+        <v>1</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="17">
+        <v>46.777470000000001</v>
+      </c>
+      <c r="F59" s="17">
+        <v>-117.08076</v>
+      </c>
+      <c r="G59" s="18">
+        <v>42480</v>
+      </c>
+      <c r="H59" s="18"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="17">
+        <v>2</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="17">
+        <v>46.777169999999998</v>
+      </c>
+      <c r="F60" s="17">
+        <v>-117.08083000000001</v>
+      </c>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="17">
+        <v>3</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="17">
+        <v>46.777000000000001</v>
+      </c>
+      <c r="F61" s="17">
+        <v>-117.0812</v>
+      </c>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="17">
+        <v>4</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="17">
+        <v>46.776969999999999</v>
+      </c>
+      <c r="F62" s="17">
+        <v>-117.08046</v>
+      </c>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="3">
+        <v>46.783499999999997</v>
+      </c>
+      <c r="F63" s="3">
+        <v>-117.0776</v>
+      </c>
+      <c r="G63" s="12">
+        <v>42480</v>
+      </c>
+      <c r="H63" s="12"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="3">
+        <v>2</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="3">
+        <v>46.783209999999997</v>
+      </c>
+      <c r="F64" s="3">
+        <v>-117.07751</v>
+      </c>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="3">
+        <v>3</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="3">
+        <v>46.782989999999998</v>
+      </c>
+      <c r="F65" s="3">
+        <v>-117.07785</v>
+      </c>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="3">
+        <v>4</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="3">
+        <v>46.783090000000001</v>
+      </c>
+      <c r="F66" s="3">
+        <v>-117.07711</v>
+      </c>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
     </row>
   </sheetData>
   <sortState ref="A2:F56">
     <sortCondition ref="A2:A56"/>
     <sortCondition ref="B2:B56"/>
   </sortState>
-  <mergeCells count="52">
-    <mergeCell ref="I51:I54"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I47:I50"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="I43:I46"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="G55:G58"/>
-    <mergeCell ref="H55:H58"/>
-    <mergeCell ref="G36:G42"/>
-    <mergeCell ref="H36:H42"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="G51:G54"/>
-    <mergeCell ref="H51:H54"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="G32:G35"/>
-    <mergeCell ref="H32:H35"/>
+  <mergeCells count="59">
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="G59:G62"/>
+    <mergeCell ref="H59:H62"/>
+    <mergeCell ref="G63:G66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A27"/>
+    <mergeCell ref="A28:A42"/>
+    <mergeCell ref="A43:A58"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="G4:G7"/>
     <mergeCell ref="H4:H7"/>
@@ -1752,16 +1912,32 @@
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="B47:B50"/>
     <mergeCell ref="B51:B54"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A27"/>
-    <mergeCell ref="A28:A42"/>
-    <mergeCell ref="A43:A58"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="G55:G58"/>
+    <mergeCell ref="H55:H58"/>
+    <mergeCell ref="G36:G42"/>
+    <mergeCell ref="H36:H42"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="G51:G54"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="I51:I54"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I47:I50"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="I43:I46"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="H32:H35"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add plot locations for 2016
Had to estimate locations at MMTN due to lack of GPS markers
</commit_message>
<xml_diff>
--- a/data/Plot locations.xlsx
+++ b/data/Plot locations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -106,12 +106,21 @@
   </si>
   <si>
     <t>This file doesn't have an easily-exportable format yet. It's not really worthwhile to export to other than KML, GeoJSON, GeoRSS or some other GIS-oriented format though, and a KML equivalent already exists…</t>
+  </si>
+  <si>
+    <t>Locations inferred from GPS tracks; removal date estimated; field harvest est. Oct 1st week</t>
+  </si>
+  <si>
+    <t>Removal date estimated; field shutdown Aug 15, harvested Aug 17</t>
+  </si>
+  <si>
+    <t>Removal date estimated; field shutdown &amp; harvested Aug 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
@@ -200,32 +209,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,9 +543,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="H63" sqref="H63:H66"/>
     </sheetView>
   </sheetViews>
@@ -554,17 +563,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -596,10 +605,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="11">
         <v>2012</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="3">
@@ -614,19 +623,19 @@
       <c r="F4" s="3">
         <v>-117.08089</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="13">
         <v>41046</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="13">
         <v>41138</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="3">
         <v>2</v>
       </c>
@@ -639,13 +648,13 @@
       <c r="F5" s="3">
         <v>-117.08078999999999</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="10"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="3">
         <v>3</v>
       </c>
@@ -658,13 +667,13 @@
       <c r="F6" s="3">
         <v>-117.08054</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="10"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="3">
         <v>4</v>
       </c>
@@ -677,12 +686,12 @@
       <c r="F7" s="3">
         <v>-117.08132000000001</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="10"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
@@ -698,15 +707,15 @@
       <c r="F8" s="1">
         <v>-117.07777</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="16">
         <v>41046</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="16">
         <v>41138</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="15"/>
       <c r="C9" s="1">
         <v>2</v>
@@ -720,11 +729,11 @@
       <c r="F9" s="1">
         <v>-117.07767</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="15"/>
       <c r="C10" s="1">
         <v>3</v>
@@ -738,11 +747,11 @@
       <c r="F10" s="1">
         <v>-117.07746</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="15"/>
       <c r="C11" s="1">
         <v>4</v>
@@ -756,14 +765,14 @@
       <c r="F11" s="1">
         <v>-117.07822</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>2013</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3">
@@ -778,16 +787,16 @@
       <c r="F12" s="3">
         <v>-117.08068</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="13">
         <v>41453</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="13">
         <v>41528</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
-      <c r="B13" s="14"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3">
         <v>2</v>
       </c>
@@ -800,12 +809,12 @@
       <c r="F13" s="3">
         <v>-117.08068</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="3">
         <v>3</v>
       </c>
@@ -818,12 +827,12 @@
       <c r="F14" s="3">
         <v>-117.08110000000001</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="3">
         <v>4</v>
       </c>
@@ -836,8 +845,8 @@
       <c r="F15" s="3">
         <v>-117.08029000000001</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
@@ -856,10 +865,10 @@
       <c r="F16" s="1">
         <v>-117.07765000000001</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="16">
         <v>41453</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="16">
         <v>41528</v>
       </c>
     </row>
@@ -878,8 +887,8 @@
       <c r="F17" s="1">
         <v>-117.07765000000001</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
@@ -896,8 +905,8 @@
       <c r="F18" s="1">
         <v>-117.07805</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
@@ -914,12 +923,12 @@
       <c r="F19" s="1">
         <v>-117.07738999999999</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="3">
@@ -934,19 +943,19 @@
       <c r="F20" s="3">
         <v>-118.59832</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="13">
         <v>41408</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="13">
         <v>41487</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
-      <c r="B21" s="14"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="3">
         <v>2</v>
       </c>
@@ -959,13 +968,13 @@
       <c r="F21" s="3">
         <v>-118.59828</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="10"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="17"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="3">
         <v>3</v>
       </c>
@@ -978,13 +987,13 @@
       <c r="F22" s="3">
         <v>-118.59793000000001</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="10"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
-      <c r="B23" s="14"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="3">
         <v>4</v>
       </c>
@@ -997,9 +1006,9 @@
       <c r="F23" s="3">
         <v>-118.59872</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="10"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="17"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
@@ -1018,13 +1027,13 @@
       <c r="F24" s="1">
         <v>-116.94855</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="16">
         <v>41415</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="16">
         <v>41506</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1043,9 +1052,9 @@
       <c r="F25" s="1">
         <v>-116.94853999999999</v>
       </c>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="10"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
@@ -1062,9 +1071,9 @@
       <c r="F26" s="1">
         <v>-116.94815</v>
       </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="10"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
@@ -1081,15 +1090,15 @@
       <c r="F27" s="1">
         <v>-116.94896</v>
       </c>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="10"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="17"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
+      <c r="A28" s="11">
         <v>2014</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="3">
@@ -1104,19 +1113,19 @@
       <c r="F28" s="3">
         <v>-117.08078</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="13">
         <v>41748</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="13">
         <v>41853</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="3">
         <v>2</v>
       </c>
@@ -1129,13 +1138,13 @@
       <c r="F29" s="3">
         <v>-117.08089</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="10"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="3">
         <v>3</v>
       </c>
@@ -1148,13 +1157,13 @@
       <c r="F30" s="3">
         <v>-117.08138</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="10"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="3">
         <v>4</v>
       </c>
@@ -1167,12 +1176,12 @@
       <c r="F31" s="3">
         <v>-117.08051</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="10"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="15" t="s">
         <v>9</v>
       </c>
@@ -1188,18 +1197,18 @@
       <c r="F32" s="1">
         <v>-117.07764</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="16">
         <v>41748</v>
       </c>
-      <c r="H32" s="13">
+      <c r="H32" s="16">
         <v>41853</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I32" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="15"/>
       <c r="C33" s="1">
         <v>2</v>
@@ -1213,12 +1222,12 @@
       <c r="F33" s="1">
         <v>-117.07767</v>
       </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="10"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="15"/>
       <c r="C34" s="1">
         <v>3</v>
@@ -1232,12 +1241,12 @@
       <c r="F34" s="1">
         <v>-117.07813</v>
       </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="10"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="17"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="15"/>
       <c r="C35" s="1">
         <v>4</v>
@@ -1251,13 +1260,13 @@
       <c r="F35" s="1">
         <v>-117.0775</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="10"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="3">
@@ -1272,16 +1281,16 @@
       <c r="F36" s="3">
         <v>-116.94868</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="13">
         <v>41813</v>
       </c>
-      <c r="H36" s="12">
+      <c r="H36" s="13">
         <v>41857</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="3">
         <v>2</v>
       </c>
@@ -1294,12 +1303,12 @@
       <c r="F37" s="3">
         <v>-116.94832</v>
       </c>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="3">
         <v>3</v>
       </c>
@@ -1312,12 +1321,12 @@
       <c r="F38" s="3">
         <v>-116.94914</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="3">
         <v>4</v>
       </c>
@@ -1330,12 +1339,12 @@
       <c r="F39" s="3">
         <v>-116.94839</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="3" t="s">
         <v>11</v>
       </c>
@@ -1348,12 +1357,12 @@
       <c r="F40" s="3">
         <v>-116.94785</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="3" t="s">
         <v>12</v>
       </c>
@@ -1366,12 +1375,12 @@
       <c r="F41" s="3">
         <v>-116.94764000000001</v>
       </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="3" t="s">
         <v>13</v>
       </c>
@@ -1384,8 +1393,8 @@
       <c r="F42" s="3">
         <v>-116.94743</v>
       </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
@@ -1406,13 +1415,13 @@
       <c r="F43" s="1">
         <v>-117.08078</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="16">
         <v>42142</v>
       </c>
-      <c r="H43" s="13">
+      <c r="H43" s="16">
         <v>42226</v>
       </c>
-      <c r="I43" s="10" t="s">
+      <c r="I43" s="17" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1431,9 +1440,9 @@
       <c r="F44" s="1">
         <v>-117.08083000000001</v>
       </c>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="10"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="17"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
@@ -1450,9 +1459,9 @@
       <c r="F45" s="1">
         <v>-117.08125</v>
       </c>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="10"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="17"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
@@ -1469,13 +1478,13 @@
       <c r="F46" s="1">
         <v>-117.08045</v>
       </c>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="10"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="17"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="3">
@@ -1490,19 +1499,19 @@
       <c r="F47" s="3">
         <v>-117.07762</v>
       </c>
-      <c r="G47" s="12">
+      <c r="G47" s="13">
         <v>42142</v>
       </c>
-      <c r="H47" s="12">
+      <c r="H47" s="13">
         <v>42226</v>
       </c>
-      <c r="I47" s="10" t="s">
+      <c r="I47" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
-      <c r="B48" s="14"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="3">
         <v>2</v>
       </c>
@@ -1515,13 +1524,13 @@
       <c r="F48" s="3">
         <v>-117.07758</v>
       </c>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="10"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="17"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
-      <c r="B49" s="14"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="3">
         <v>3</v>
       </c>
@@ -1534,13 +1543,13 @@
       <c r="F49" s="3">
         <v>-117.07792999999999</v>
       </c>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="10"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="17"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="B50" s="14"/>
+      <c r="B50" s="11"/>
       <c r="C50" s="3">
         <v>4</v>
       </c>
@@ -1553,9 +1562,9 @@
       <c r="F50" s="3">
         <v>-117.07735</v>
       </c>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="10"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="17"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="15"/>
@@ -1574,13 +1583,13 @@
       <c r="F51" s="1">
         <v>-118.59838999999999</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="16">
         <v>42082</v>
       </c>
-      <c r="H51" s="13">
+      <c r="H51" s="16">
         <v>42194</v>
       </c>
-      <c r="I51" s="10" t="s">
+      <c r="I51" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1599,9 +1608,9 @@
       <c r="F52" s="1">
         <v>-118.5984</v>
       </c>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="10"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="17"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
@@ -1618,9 +1627,9 @@
       <c r="F53" s="1">
         <v>-118.59878999999999</v>
       </c>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="10"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="17"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
@@ -1637,13 +1646,13 @@
       <c r="F54" s="1">
         <v>-118.59805</v>
       </c>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="10"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="17"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C55" s="3">
@@ -1658,16 +1667,16 @@
       <c r="F55" s="3">
         <v>-116.94859</v>
       </c>
-      <c r="G55" s="12">
+      <c r="G55" s="13">
         <v>42090</v>
       </c>
-      <c r="H55" s="12">
+      <c r="H55" s="13">
         <v>42219</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
-      <c r="B56" s="14"/>
+      <c r="B56" s="11"/>
       <c r="C56" s="3">
         <v>2</v>
       </c>
@@ -1680,12 +1689,12 @@
       <c r="F56" s="3">
         <v>-116.94879</v>
       </c>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
-      <c r="B57" s="14"/>
+      <c r="B57" s="11"/>
       <c r="C57" s="3">
         <v>3</v>
       </c>
@@ -1698,12 +1707,12 @@
       <c r="F57" s="3">
         <v>-116.94925000000001</v>
       </c>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
-      <c r="B58" s="14"/>
+      <c r="B58" s="11"/>
       <c r="C58" s="3">
         <v>4</v>
       </c>
@@ -1716,90 +1725,98 @@
       <c r="F58" s="3">
         <v>-116.94855</v>
       </c>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="14">
+      <c r="A59" s="11">
         <v>2016</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="17">
+      <c r="C59" s="10">
         <v>1</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="17">
+      <c r="E59" s="10">
         <v>46.777470000000001</v>
       </c>
-      <c r="F59" s="17">
+      <c r="F59" s="10">
         <v>-117.08076</v>
       </c>
-      <c r="G59" s="18">
+      <c r="G59" s="12">
         <v>42480</v>
       </c>
-      <c r="H59" s="18"/>
+      <c r="H59" s="12">
+        <v>42590</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="17">
+      <c r="A60" s="11"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="10">
         <v>2</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="10">
         <v>46.777169999999998</v>
       </c>
-      <c r="F60" s="17">
+      <c r="F60" s="10">
         <v>-117.08083000000001</v>
       </c>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="17"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="17">
+      <c r="A61" s="11"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="10">
         <v>3</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="17">
+      <c r="E61" s="10">
         <v>46.777000000000001</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="10">
         <v>-117.0812</v>
       </c>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="17"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17">
-        <v>4</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" s="17">
+      <c r="A62" s="11"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="10">
+        <v>4</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="10">
         <v>46.776969999999999</v>
       </c>
-      <c r="F62" s="17">
+      <c r="F62" s="10">
         <v>-117.08046</v>
       </c>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="17"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14" t="s">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="3">
@@ -1814,14 +1831,19 @@
       <c r="F63" s="3">
         <v>-117.0776</v>
       </c>
-      <c r="G63" s="12">
+      <c r="G63" s="13">
         <v>42480</v>
       </c>
-      <c r="H63" s="12"/>
+      <c r="H63" s="13">
+        <v>42597</v>
+      </c>
+      <c r="I63" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
       <c r="C64" s="3">
         <v>2</v>
       </c>
@@ -1834,12 +1856,13 @@
       <c r="F64" s="3">
         <v>-117.07751</v>
       </c>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="17"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
       <c r="C65" s="3">
         <v>3</v>
       </c>
@@ -1852,12 +1875,13 @@
       <c r="F65" s="3">
         <v>-117.07785</v>
       </c>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
       <c r="C66" s="3">
         <v>4</v>
       </c>
@@ -1870,58 +1894,107 @@
       <c r="F66" s="3">
         <v>-117.07711</v>
       </c>
-      <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="17"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+      <c r="B67" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="1">
+        <v>46.757620000000003</v>
+      </c>
+      <c r="F67" s="1">
+        <v>-116.94869</v>
+      </c>
+      <c r="G67" s="16">
+        <v>42492</v>
+      </c>
+      <c r="H67" s="16">
+        <v>42643</v>
+      </c>
+      <c r="I67" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="1">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="1">
+        <v>46.757339999999999</v>
+      </c>
+      <c r="F68" s="1">
+        <v>-116.94875999999999</v>
+      </c>
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="17"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="1">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="1">
+        <v>46.757150000000003</v>
+      </c>
+      <c r="F69" s="1">
+        <v>-116.94851</v>
+      </c>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="17"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="1">
+        <v>4</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70" s="1">
+        <v>46.757330000000003</v>
+      </c>
+      <c r="F70" s="1">
+        <v>-116.94916000000001</v>
+      </c>
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+      <c r="I70" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A2:F56">
     <sortCondition ref="A2:A56"/>
     <sortCondition ref="B2:B56"/>
   </sortState>
-  <mergeCells count="59">
-    <mergeCell ref="A59:A66"/>
-    <mergeCell ref="G59:G62"/>
-    <mergeCell ref="H59:H62"/>
-    <mergeCell ref="G63:G66"/>
-    <mergeCell ref="H63:H66"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="A12:A27"/>
-    <mergeCell ref="A28:A42"/>
-    <mergeCell ref="A43:A58"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B36:B42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="G55:G58"/>
-    <mergeCell ref="H55:H58"/>
-    <mergeCell ref="G36:G42"/>
-    <mergeCell ref="H36:H42"/>
-    <mergeCell ref="G43:G46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="G51:G54"/>
-    <mergeCell ref="H51:H54"/>
+  <mergeCells count="65">
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="A59:A70"/>
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="G67:G70"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="I59:I62"/>
+    <mergeCell ref="I63:I66"/>
     <mergeCell ref="I51:I54"/>
     <mergeCell ref="I24:I27"/>
     <mergeCell ref="A1:I1"/>
@@ -1938,6 +2011,48 @@
     <mergeCell ref="H28:H31"/>
     <mergeCell ref="G32:G35"/>
     <mergeCell ref="H32:H35"/>
+    <mergeCell ref="G55:G58"/>
+    <mergeCell ref="H55:H58"/>
+    <mergeCell ref="G36:G42"/>
+    <mergeCell ref="H36:H42"/>
+    <mergeCell ref="G43:G46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="G51:G54"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="A12:A27"/>
+    <mergeCell ref="A28:A42"/>
+    <mergeCell ref="A43:A58"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B36:B42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="G59:G62"/>
+    <mergeCell ref="H59:H62"/>
+    <mergeCell ref="G63:G66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B66"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>